<commit_message>
finished routes and added auth by userid
</commit_message>
<xml_diff>
--- a/DisenoAPIBedushop.xlsx
+++ b/DisenoAPIBedushop.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FoodLovers\Desktop\Courses\02 Bedu\15 BeduShop-Backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C21F42-C615-4C98-91C2-E935D60A153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28830" yWindow="30" windowWidth="21300" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,363 +25,357 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="97">
-  <si>
-    <t xml:space="preserve">Path version 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/api/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comentario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">products/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get product for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seller,Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create new product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update product for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart_Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PATCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart_Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DELETE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete product for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se considera inecesaria ya que no debe haber borrado de productos, sino cambio de estatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart_Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categories/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get category for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create new category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update category for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete category for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Userid,Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">users/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get user for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Userid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create new user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update user for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete user for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reviews/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get review for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create new review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update review for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se considera innecesaria ya que por lo regular un review solo es creado, pero no editado por el usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete review for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all products in cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cart/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get product in cart for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buyer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cart/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add new product at cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update product in cart for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order, Order-details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orders/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get orders for user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orders/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get order for given Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checkout cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Una vez generada la order, no es posible editar completamente la orden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Una vez generada la order, no es posible eliminar la orden, solo cambiar su estatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orders/products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all products in orders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get all userTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Usertype by Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create new userType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDATE userTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DELETE UserType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID endpoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requerimiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, 25-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usuario de BeduShop, Quiero ver todos los productos en venta para elegir los que me interesan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como Vendedor Quiero poder publicar mis productos para que los demas usarios pueden compar mis productos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usario de BeduShop, Quiero ver todos los comentarios y reseñas sobre los productos para poder tomar una decicion informada antes de hacer una compra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usario quiero ver todos los productos que eh comprado para poder llevar un registro si se me entrego</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usario quiero ver un historial de mis compras para poder llevar un registro de cuanto me costo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como Vendedor quiero poder agregar informacion sobre mi producto para que los usarios me puedan encontrar mas facil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usario quiero poder filtrar los productos para poder encontrar justamente lo que busco y no sentirme abrubado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">como vendedor quiero poder eliminar productos para que generar alguna confusion con los productos que ya no manejo.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="98">
+  <si>
+    <t>Path version 1</t>
+  </si>
+  <si>
+    <t>Permits</t>
+  </si>
+  <si>
+    <t>/api/v1/</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>Get all products</t>
+  </si>
+  <si>
+    <t>Cart_ID</t>
+  </si>
+  <si>
+    <t>products/{id}</t>
+  </si>
+  <si>
+    <t>Get product for given Id</t>
+  </si>
+  <si>
+    <t>Product_ID</t>
+  </si>
+  <si>
+    <t>Seller,Admin</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Create new product</t>
+  </si>
+  <si>
+    <t>User_ID</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Update product for given Id</t>
+  </si>
+  <si>
+    <t>Cart_Date</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>Cart_Quantity</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Delete product for given Id</t>
+  </si>
+  <si>
+    <t>Se considera inecesaria ya que no debe haber borrado de productos, sino cambio de estatus</t>
+  </si>
+  <si>
+    <t>Cart_Price</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>Get all categories</t>
+  </si>
+  <si>
+    <t>categories/{id}</t>
+  </si>
+  <si>
+    <t>Get category for given Id</t>
+  </si>
+  <si>
+    <t>Create new category</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Update category for given Id</t>
+  </si>
+  <si>
+    <t>Delete category for given Id</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>Get all users</t>
+  </si>
+  <si>
+    <t>Userid,Admin</t>
+  </si>
+  <si>
+    <t>users/{id}</t>
+  </si>
+  <si>
+    <t>Get user for given Id</t>
+  </si>
+  <si>
+    <t>Userid</t>
+  </si>
+  <si>
+    <t>Create new user</t>
+  </si>
+  <si>
+    <t>Update user for given Id</t>
+  </si>
+  <si>
+    <t>Delete user for given Id</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>Get all reviews</t>
+  </si>
+  <si>
+    <t>reviews/{id}</t>
+  </si>
+  <si>
+    <t>Get review for given Id</t>
+  </si>
+  <si>
+    <t>Create new review</t>
+  </si>
+  <si>
+    <t>Update review for given Id</t>
+  </si>
+  <si>
+    <t>Se considera innecesaria ya que por lo regular un review solo es creado, pero no editado por el usuario</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Delete review for given Id</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>Get all products in cart</t>
+  </si>
+  <si>
+    <t>cart/{id}</t>
+  </si>
+  <si>
+    <t>Get product in cart for given Id</t>
+  </si>
+  <si>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>cart/</t>
+  </si>
+  <si>
+    <t>Add new product at cart</t>
+  </si>
+  <si>
+    <t>Update product in cart for given Id</t>
+  </si>
+  <si>
+    <t>Order, Order-details</t>
+  </si>
+  <si>
+    <t>orders/</t>
+  </si>
+  <si>
+    <t>Get orders for user</t>
+  </si>
+  <si>
+    <t>orders/{id}</t>
+  </si>
+  <si>
+    <t>Get order for given Id</t>
+  </si>
+  <si>
+    <t>Checkout cart</t>
+  </si>
+  <si>
+    <t>Una vez generada la order, no es posible editar completamente la orden</t>
+  </si>
+  <si>
+    <t>Una vez generada la order, no es posible eliminar la orden, solo cambiar su estatus</t>
+  </si>
+  <si>
+    <t>orders/products</t>
+  </si>
+  <si>
+    <t>Get all products in orders</t>
+  </si>
+  <si>
+    <t>userTypes</t>
+  </si>
+  <si>
+    <t>Get all userTypes</t>
+  </si>
+  <si>
+    <t>Get Usertype by Id</t>
+  </si>
+  <si>
+    <t>Create new userType</t>
+  </si>
+  <si>
+    <t>UPDATE userTypes</t>
+  </si>
+  <si>
+    <t>DELETE UserType</t>
+  </si>
+  <si>
+    <t>ID endpoint</t>
+  </si>
+  <si>
+    <t>Requerimiento</t>
+  </si>
+  <si>
+    <t>1, 25-30</t>
+  </si>
+  <si>
+    <t>Como usuario de BeduShop, Quiero ver todos los productos en venta para elegir los que me interesan</t>
+  </si>
+  <si>
+    <t>Como Vendedor Quiero poder publicar mis productos para que los demas usarios pueden compar mis productos</t>
+  </si>
+  <si>
+    <t>19-24</t>
+  </si>
+  <si>
+    <t>Como usario de BeduShop, Quiero ver todos los comentarios y reseñas sobre los productos para poder tomar una decicion informada antes de hacer una compra</t>
+  </si>
+  <si>
+    <t>Como usario quiero ver todos los productos que eh comprado para poder llevar un registro si se me entrego</t>
+  </si>
+  <si>
+    <t>Como usario quiero ver un historial de mis compras para poder llevar un registro de cuanto me costo</t>
+  </si>
+  <si>
+    <t>Como Vendedor quiero poder agregar informacion sobre mi producto para que los usarios me puedan encontrar mas facil</t>
+  </si>
+  <si>
+    <t>Como usario quiero poder filtrar los productos para poder encontrar justamente lo que busco y no sentirme abrubado</t>
+  </si>
+  <si>
+    <t>como vendedor quiero poder eliminar productos para que generar alguna confusion con los productos que ya no manejo.</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-m"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\-m"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <strike val="true"/>
+      <strike/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,133 +412,97 @@
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -598,31 +561,340 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.87"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -642,7 +914,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -656,7 +928,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -682,8 +954,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -704,12 +976,15 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -730,12 +1005,15 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -756,38 +1034,42 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
+      <c r="J6" t="s">
+        <v>97</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -808,12 +1090,15 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -831,17 +1116,20 @@
       <c r="F9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="K9" s="9" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -862,9 +1150,12 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -885,9 +1176,12 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="J11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -908,38 +1202,40 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" t="s">
+        <v>97</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -960,12 +1256,14 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="n">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -983,17 +1281,19 @@
       <c r="F15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1014,14 +1314,14 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J16" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1042,61 +1342,66 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
+      <c r="J17" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="n">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="n">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="22"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="n">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1117,11 +1422,14 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
+      <c r="J20" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="n">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1139,16 +1447,19 @@
       <c r="F21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1169,11 +1480,14 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
+      <c r="J22" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1194,11 +1508,14 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
+      <c r="J23" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1219,40 +1536,42 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="J24" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="n">
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>22</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="n">
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1270,17 +1589,19 @@
       <c r="F26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1301,12 +1622,14 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="n">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1327,12 +1650,14 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="n">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1353,12 +1678,14 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="n">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1379,38 +1706,40 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="n">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
         <v>28</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="n">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1431,12 +1760,14 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="n">
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1457,12 +1788,14 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="n">
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1483,12 +1816,14 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="n">
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1509,12 +1844,14 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="n">
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1535,40 +1872,42 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="n">
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
         <v>34</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="1"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="n">
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1589,12 +1928,14 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="n">
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
         <v>36</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1612,42 +1953,42 @@
       <c r="F39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="n">
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
         <v>37</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G40" s="9"/>
+      <c r="G40" s="8"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>79</v>
@@ -1665,11 +2006,13 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>79</v>
@@ -1687,11 +2030,13 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="J42" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>79</v>
@@ -1709,33 +2054,37 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="J43" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="21"/>
+      <c r="F44" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>79</v>
@@ -1753,11 +2102,13 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="J45" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>79</v>
@@ -1775,18 +2126,20 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
+      <c r="J46" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="15"/>
+      <c r="C47" s="14"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -1796,7 +2149,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>87</v>
       </c>
@@ -1814,8 +2167,8 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="16" t="n">
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
         <v>44713</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1832,7 +2185,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
@@ -1842,8 +2195,8 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>37</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1852,8 +2205,8 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1862,8 +2215,8 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="16" t="n">
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
         <v>44713</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1872,8 +2225,8 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1882,32 +2235,27 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="n">
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
         <v>5</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G15:I15"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G15:J15"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G25:K25"/>
     <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G39:J39"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>